<commit_message>
Updated Gantt chart on Project Plan
</commit_message>
<xml_diff>
--- a/docs/Review/to review/Gantt chart.xlsx
+++ b/docs/Review/to review/Gantt chart.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Task ID</t>
   </si>
@@ -114,6 +113,27 @@
   </si>
   <si>
     <t>SE_05_QA_01/02/03/04/05</t>
+  </si>
+  <si>
+    <t>High level design</t>
+  </si>
+  <si>
+    <t>Deliverable key:</t>
+  </si>
+  <si>
+    <t>Test specification</t>
+  </si>
+  <si>
+    <t>Design specification</t>
+  </si>
+  <si>
+    <t>1st Prototype</t>
+  </si>
+  <si>
+    <t>Delivery of software</t>
+  </si>
+  <si>
+    <t>Documentation handover</t>
   </si>
 </sst>
 </file>
@@ -142,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,30 +171,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -182,28 +232,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +736,7 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+      <selection activeCell="S32" sqref="A1:S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,44 +757,46 @@
       <c r="B2" s="2">
         <v>42296</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>42303</v>
       </c>
       <c r="D2" s="2">
         <v>42310</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>42317</v>
       </c>
       <c r="F2" s="2">
         <v>42324</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="7">
         <v>42331</v>
       </c>
       <c r="H2" s="2">
         <v>42338</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="8">
         <v>42345</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>42352</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="2">
+      <c r="K2" s="3">
+        <v>42359</v>
+      </c>
+      <c r="L2" s="3">
         <v>42366</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="3">
         <v>42373</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <v>42380</v>
       </c>
       <c r="O2" s="2">
         <v>42387</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="45">
         <v>42394</v>
       </c>
       <c r="Q2" s="2">
@@ -575,291 +805,715 @@
       <c r="R2" s="2">
         <v>42408</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="46">
         <v>42415</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="H3" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="30"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="K4" s="5"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="35"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="K5" s="5"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="34"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="K6" s="5"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="34"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="K7" s="5"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="34"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
-      <c r="K8" s="5"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="34"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="K9" s="5"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="34"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="K10" s="5"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="K11" s="5"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="K12" s="5"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="26"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="26"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="7"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="26"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="26"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="26"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="26"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="26"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="26"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="26"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="5"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K27" s="5"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="26"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K28" s="5"/>
-      <c r="P28" s="7"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K29" s="5"/>
-      <c r="P29" s="7"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="5"/>
-      <c r="P30" s="7"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="26"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="5"/>
-      <c r="P31" s="7"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="5"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>